<commit_message>
updates ENV unit new data
</commit_message>
<xml_diff>
--- a/static/download/xls/CO2_emissions_by_state.xlsx
+++ b/static/download/xls/CO2_emissions_by_state.xlsx
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -380,9 +380,6 @@
     <t>CO2 (MTonnes)</t>
   </si>
   <si>
-    <t>EUROCONTROL - Environment Unit</t>
-  </si>
-  <si>
     <t>Please select state</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>traffic for the entire year (for that state)</t>
+  </si>
+  <si>
+    <t>EUROCONTROL Aviation Sustainability Unit</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1556,6 @@
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1631,7 +1630,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2860,7 +2858,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1200"/>
-            <a:t>This data is provided by the EUROCONTROL Environment Unit in the interest of the exchange of information. It may be copied in whole or in part providing that this copyright notice and disclaimer are included. The information may not be modified without prior written permission from  EUROCONTROL.</a:t>
+            <a:t>This data is supplied by the EUROCONTROL Aviation Sustainability Unit in the interest of the exchange of information. It may be copied in whole or in part providing that this copyright notice and disclaimer are included. The information may not be modified without prior written permission from  EUROCONTROL.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7427,7 +7425,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="B4:D14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -8266,7 +8264,7 @@
   <dimension ref="E1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8296,7 +8294,7 @@
   <dimension ref="B2:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8313,7 +8311,7 @@
         <v>104</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="18"/>
@@ -8428,7 +8426,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="22">
         <v>10468</v>
@@ -15923,7 +15921,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -15945,10 +15943,10 @@
         <v>114</v>
       </c>
       <c r="E4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>